<commit_message>
Added reshaping steps for SAHFOS Data. Split documentation into readme's specific to the sources. Stopped cleanup before unit conversions
</commit_message>
<xml_diff>
--- a/data_raw/SAHFOS-MBA_2013-2017/MC part1.xlsx
+++ b/data_raw/SAHFOS-MBA_2013-2017/MC part1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apershing/Dropbox/Work/Projects/CafeGOM/Zooplankton/CPR/SAHFOS_2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akemberling/Documents/Repositories/NERACOOS_CPR_DATA/data_raw/SAHFOS-MBA_2013-2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D8898C-CD04-094E-971A-5C5351EDAE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25740" windowHeight="22600" tabRatio="722" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="722" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phyto" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="taxa list-trav" sheetId="10" r:id="rId6"/>
     <sheet name="taxa list-eye" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="330">
   <si>
     <t>Sample_Id</t>
   </si>
@@ -1021,11 +1022,14 @@
   <si>
     <t>included in 90</t>
   </si>
+  <si>
+    <t>note</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1826,7 +1830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK165"/>
   <sheetViews>
     <sheetView topLeftCell="A147" workbookViewId="0">
@@ -1835,9 +1839,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33362,7 +33366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV165"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
@@ -33371,7 +33375,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
@@ -57471,11 +57475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -83559,18 +83563,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B58"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="10" max="10" width="33.59765625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -84655,29 +84659,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>173</v>
       </c>
@@ -84685,7 +84692,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -84693,7 +84700,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -84701,7 +84708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -84709,7 +84716,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>177</v>
       </c>
@@ -84717,7 +84724,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -84725,7 +84732,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -84733,7 +84740,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -84741,7 +84748,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -84749,7 +84756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -84757,7 +84764,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -84765,7 +84772,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -84773,7 +84780,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -84781,7 +84788,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -85131,11 +85138,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C48"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85152,6 +85159,9 @@
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -85569,29 +85579,32 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -85599,7 +85612,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -85607,7 +85620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -85615,7 +85628,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -85623,7 +85636,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -85631,7 +85644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>235</v>
       </c>
@@ -85639,7 +85652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>236</v>
       </c>
@@ -85647,7 +85660,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -85655,7 +85668,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>238</v>
       </c>
@@ -85663,7 +85676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -85671,7 +85684,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>240</v>
       </c>
@@ -85679,7 +85692,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>241</v>
       </c>
@@ -85687,7 +85700,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -85695,7 +85708,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>243</v>
       </c>

</xml_diff>

<commit_message>
Adding Adam's changes back in
</commit_message>
<xml_diff>
--- a/data_raw/SAHFOS-MBA_2013-2017/MC part1.xlsx
+++ b/data_raw/SAHFOS-MBA_2013-2017/MC part1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apershing/Dropbox/Work/Projects/CafeGOM/Zooplankton/CPR/SAHFOS_2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akemberling/Documents/Repositories/NERACOOS_CPR_DATA/data_raw/SAHFOS-MBA_2013-2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D8898C-CD04-094E-971A-5C5351EDAE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25740" windowHeight="22600" tabRatio="722" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="722" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phyto" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="taxa list-trav" sheetId="10" r:id="rId6"/>
     <sheet name="taxa list-eye" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="330">
   <si>
     <t>Sample_Id</t>
   </si>
@@ -1021,11 +1022,14 @@
   <si>
     <t>included in 90</t>
   </si>
+  <si>
+    <t>note</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1826,7 +1830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK165"/>
   <sheetViews>
     <sheetView topLeftCell="A147" workbookViewId="0">
@@ -1835,9 +1839,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33362,7 +33366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV165"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
@@ -33371,7 +33375,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
@@ -57471,11 +57475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -83559,18 +83563,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B58"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="10" max="10" width="33.59765625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -84655,29 +84659,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>173</v>
       </c>
@@ -84685,7 +84692,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -84693,7 +84700,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -84701,7 +84708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -84709,7 +84716,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>177</v>
       </c>
@@ -84717,7 +84724,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -84725,7 +84732,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -84733,7 +84740,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -84741,7 +84748,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -84749,7 +84756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -84757,7 +84764,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -84765,7 +84772,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -84773,7 +84780,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -84781,7 +84788,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -85131,11 +85138,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C48"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85152,6 +85159,9 @@
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -85569,29 +85579,32 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>172</v>
       </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -85599,7 +85612,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -85607,7 +85620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -85615,7 +85628,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -85623,7 +85636,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -85631,7 +85644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>235</v>
       </c>
@@ -85639,7 +85652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>236</v>
       </c>
@@ -85647,7 +85660,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -85655,7 +85668,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>238</v>
       </c>
@@ -85663,7 +85676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -85671,7 +85684,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>240</v>
       </c>
@@ -85679,7 +85692,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>241</v>
       </c>
@@ -85687,7 +85700,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -85695,7 +85708,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>243</v>
       </c>

</xml_diff>